<commit_message>
Using Formulas in Data Validation
</commit_message>
<xml_diff>
--- a/Intermediate II/Week 1/workbook/W1_V3 FormulasInDataValidation.xlsx
+++ b/Intermediate II/Week 1/workbook/W1_V3 FormulasInDataValidation.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mq20084022\Google Drive\Excel MOOC\003 Course 3 - Intermediate II\01 Week 1\01 Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate II\Week 1\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F882DB58-91C6-4B60-96B7-79B831D77BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9168"/>
+    <workbookView xWindow="9130" yWindow="200" windowWidth="10070" windowHeight="9490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="BATH_020">Inventory!$A$5:$A$55</definedName>
     <definedName name="Departments">Lists!$C$4:$C$9</definedName>
     <definedName name="Origins">Lists!$E$4:$E$12</definedName>
+    <definedName name="Product_Code">Inventory!$A$4:$A$55</definedName>
     <definedName name="Suppliers">Lists!$A$4:$A$10</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -467,10 +470,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="00"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -551,7 +555,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -576,6 +580,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -584,34 +589,13 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -636,6 +620,27 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -650,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Inventory" displayName="Inventory" ref="A3:M54" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" headerRowCellStyle="Heading 3">
-  <autoFilter ref="A3:M54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Inventory" displayName="Inventory" ref="A3:M55" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" headerRowCellStyle="Heading 3">
+  <autoFilter ref="A3:M55" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -667,49 +672,49 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Product Code"/>
-    <tableColumn id="2" name="Item Description"/>
-    <tableColumn id="3" name="Supplier"/>
-    <tableColumn id="4" name="Department"/>
-    <tableColumn id="5" name="Origin"/>
-    <tableColumn id="6" name="Location"/>
-    <tableColumn id="7" name="Rack" dataDxfId="9"/>
-    <tableColumn id="8" name="In Stock" dataDxfId="8"/>
-    <tableColumn id="9" name="Target Level" dataDxfId="7"/>
-    <tableColumn id="10" name="Reorder Level" dataDxfId="6"/>
-    <tableColumn id="11" name="Last Ordered" dataDxfId="5"/>
-    <tableColumn id="12" name="Unit Cost" dataDxfId="4"/>
-    <tableColumn id="13" name="Retail Price" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Product Code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item Description"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Supplier"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Department"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Origin"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Location"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Rack" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="In Stock" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Target Level" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Reorder Level" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Last Ordered" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Unit Cost" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Retail Price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="OriginsTable" displayName="OriginsTable" ref="E3:E12" totalsRowShown="0" headerRowBorderDxfId="2" headerRowCellStyle="Heading 3">
-  <autoFilter ref="E3:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="OriginsTable" displayName="OriginsTable" ref="E3:E12" totalsRowShown="0" headerRowBorderDxfId="11" headerRowCellStyle="Heading 3">
+  <autoFilter ref="E3:E12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Origins"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Origins"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SuppliersTable" displayName="SuppliersTable" ref="A3:A10" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 3">
-  <autoFilter ref="A3:A10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SuppliersTable" displayName="SuppliersTable" ref="A3:A10" totalsRowShown="0" headerRowBorderDxfId="10" headerRowCellStyle="Heading 3">
+  <autoFilter ref="A3:A10" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Suppliers"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Suppliers"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="DepartmentsTable" displayName="DepartmentsTable" ref="C3:C9" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 3">
-  <autoFilter ref="C3:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DepartmentsTable" displayName="DepartmentsTable" ref="C3:C9" totalsRowShown="0" headerRowBorderDxfId="9" headerRowCellStyle="Heading 3">
+  <autoFilter ref="C3:C9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Departments"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Departments"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1011,29 +1016,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="8.54296875" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" style="10" customWidth="1"/>
     <col min="8" max="8" width="10" style="10" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="30.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>134</v>
       </c>
@@ -1050,13 +1057,13 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
@@ -1097,7 +1104,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1302,7 +1309,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1466,7 +1473,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1548,7 +1555,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1589,7 +1596,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>10.99</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1671,7 +1678,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1753,7 +1760,7 @@
         <v>10.99</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1794,7 +1801,7 @@
         <v>7.49</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1835,7 +1842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1958,7 +1965,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -1999,7 +2006,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2040,7 +2047,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2081,7 +2088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2122,7 +2129,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2163,7 +2170,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2204,7 +2211,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2245,7 +2252,7 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2286,7 +2293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2327,7 +2334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2368,7 +2375,7 @@
         <v>108.97</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2409,7 +2416,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -2491,7 +2498,7 @@
         <v>97.99</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2573,7 +2580,7 @@
         <v>107.712</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>87.516000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2655,7 +2662,7 @@
         <v>125.664</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -2696,7 +2703,7 @@
         <v>171.666</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2737,7 +2744,7 @@
         <v>117.81</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -2778,7 +2785,7 @@
         <v>102.102</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -2819,7 +2826,7 @@
         <v>109.956</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -2860,7 +2867,7 @@
         <v>139.12799999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2901,7 +2908,7 @@
         <v>109.956</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -2942,7 +2949,7 @@
         <v>87.516000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -2983,7 +2990,7 @@
         <v>170.54400000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -3024,7 +3031,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -3065,7 +3072,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -3106,7 +3113,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -3147,7 +3154,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -3188,26 +3195,35 @@
         <v>830</v>
       </c>
     </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G55" s="9"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+    </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Rack Number" error="Please enter a rack number between 1 and 9" promptTitle="Rack Number" prompt="Please enter a rack number between 1 and 9" sqref="G4:G54">
+  <dataValidations count="7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Rack Number" error="Please enter a rack number between 1 and 9" promptTitle="Rack Number" prompt="Please enter a rack number between 1 and 9" sqref="G4:G55" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
       <formula2>9</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Code" error="Should be 8 characters_x000a_" sqref="A4:A54">
-      <formula1>8</formula1>
+    <dataValidation type="custom" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Code" error="Duplicated product code is not accepted._x000a_" sqref="A4:A55" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>COUNTIFS(Product_Code,A4)&lt;=1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F55" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Basement,Showroom"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E55" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>Origins</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C55" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>Suppliers</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D55" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>Departments</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K55" xr:uid="{E3E34D01-BB5F-4651-9130-6E9B9C182015}">
+      <formula1>TODAY()</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3219,21 +3235,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -3242,8 +3258,8 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
@@ -3254,7 +3270,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -3265,7 +3281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -3276,7 +3292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -3287,7 +3303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -3298,7 +3314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -3309,7 +3325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -3320,7 +3336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -3328,12 +3344,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
Working with Data Validation
</commit_message>
<xml_diff>
--- a/Intermediate II/Week 1/workbook/W1_V3 FormulasInDataValidation.xlsx
+++ b/Intermediate II/Week 1/workbook/W1_V3 FormulasInDataValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate II\Week 1\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F882DB58-91C6-4B60-96B7-79B831D77BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4005AED8-EEBB-4A2F-8901-52CEA71551DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9130" yWindow="200" windowWidth="10070" windowHeight="9490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9470" yWindow="540" windowWidth="10070" windowHeight="9490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -589,6 +589,27 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
@@ -620,27 +641,6 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -655,7 +655,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Inventory" displayName="Inventory" ref="A3:M55" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Inventory" displayName="Inventory" ref="A3:M55" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" headerRowCellStyle="Heading 3">
   <autoFilter ref="A3:M55" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -678,20 +678,20 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Department"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Origin"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Location"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Rack" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="In Stock" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Target Level" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Reorder Level" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Last Ordered" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Unit Cost" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Retail Price" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Rack" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="In Stock" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Target Level" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Reorder Level" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Last Ordered" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Unit Cost" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Retail Price" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="OriginsTable" displayName="OriginsTable" ref="E3:E12" totalsRowShown="0" headerRowBorderDxfId="11" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="OriginsTable" displayName="OriginsTable" ref="E3:E12" totalsRowShown="0" headerRowBorderDxfId="2" headerRowCellStyle="Heading 3">
   <autoFilter ref="E3:E12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Origins"/>
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SuppliersTable" displayName="SuppliersTable" ref="A3:A10" totalsRowShown="0" headerRowBorderDxfId="10" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SuppliersTable" displayName="SuppliersTable" ref="A3:A10" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 3">
   <autoFilter ref="A3:A10" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Suppliers"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DepartmentsTable" displayName="DepartmentsTable" ref="C3:C9" totalsRowShown="0" headerRowBorderDxfId="9" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="DepartmentsTable" displayName="DepartmentsTable" ref="C3:C9" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 3">
   <autoFilter ref="C3:C9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Departments"/>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:A55 C4:G55 K4:K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>